<commit_message>
updated the project documents
</commit_message>
<xml_diff>
--- a/Project_Doc/Project-plan.xlsx
+++ b/Project_Doc/Project-plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Coding\AWS\AWS_project\Project_Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Coding\AWS\AWS_project\AWS_UKDER1_Rekognition\Project_Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5C277D-A393-40EC-8768-457CC6797516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2BC66B-D927-4C90-B708-068661508C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project breif" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>Starting date</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -225,6 +225,22 @@
   </si>
   <si>
     <t>4. Present the result back to the end user</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andrejz/Robert</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hassan/Mou</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Akash/Narinder</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Progress</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -526,7 +542,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -564,6 +580,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -850,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AAA790E-0128-41EF-9AA9-7614C935EF5F}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -897,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B31B63-6157-40AF-88DB-9E54A65E67A5}">
   <dimension ref="B1:F18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1094,22 +1113,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -1117,7 +1137,7 @@
         <v>44340</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>3</v>
       </c>
@@ -1125,7 +1145,7 @@
         <v>44374</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>16</v>
       </c>
@@ -1134,7 +1154,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>1</v>
       </c>
@@ -1150,8 +1170,11 @@
       <c r="E5" s="18" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
         <v>14</v>
       </c>
@@ -1159,31 +1182,35 @@
       <c r="C6" s="20"/>
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="27"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C7">
         <v>7</v>
       </c>
       <c r="D7" s="28">
-        <v>44345</v>
+        <v>44352</v>
       </c>
       <c r="E7" s="28">
         <f>IFERROR(IF(INT(C7) &gt; 0, D7+C7, "TBD"), "")</f>
-        <v>44352</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>44359</v>
+      </c>
+      <c r="F7" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C8">
         <v>14</v>
@@ -1192,16 +1219,19 @@
         <v>44338</v>
       </c>
       <c r="E8" s="28">
-        <f t="shared" ref="E8:E11" si="0">IFERROR(IF(INT(C8) &gt; 0, D8+C8, "TBD"), "")</f>
+        <f>IFERROR(IF(INT(C8) &gt; 0, D8+C8, "TBD"), "")</f>
         <v>44352</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C9">
         <v>14</v>
@@ -1210,11 +1240,14 @@
         <v>44338</v>
       </c>
       <c r="E9" s="28">
-        <f t="shared" si="0"/>
+        <f>IFERROR(IF(INT(C9) &gt; 0, D9+C9, "TBD"), "")</f>
         <v>44352</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1222,11 +1255,14 @@
         <v>11</v>
       </c>
       <c r="E10" s="28" t="str">
-        <f t="shared" si="0"/>
+        <f>IFERROR(IF(INT(C10) &gt; 0, D10+C10, "TBD"), "")</f>
         <v>TBD</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1234,11 +1270,14 @@
         <v>13</v>
       </c>
       <c r="E11" s="28" t="str">
-        <f t="shared" si="0"/>
+        <f>IFERROR(IF(INT(C11) &gt; 0, D11+C11, "TBD"), "")</f>
         <v>TBD</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>15</v>
       </c>
@@ -1246,6 +1285,7 @@
       <c r="C12" s="20"/>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>